<commit_message>
Updated Code With Item System
Items are created and system is in place for use. It's only been tested
a little bit but seems to be working.
</commit_message>
<xml_diff>
--- a/Files as of 5-31/SpecialAttacks.xlsx
+++ b/Files as of 5-31/SpecialAttacks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sierra\Documents\Post Bacc College Stuff\CSCD 349\Team Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sierra\Documents\Post Bacc College Stuff\CSCD 349\Team Project\Current Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>Good Guys</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Steal Life</t>
-  </si>
-  <si>
-    <t>yA15</t>
   </si>
   <si>
     <t>Roulette Heal</t>
@@ -481,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +530,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -606,6 +603,9 @@
       <c r="C7" t="s">
         <v>37</v>
       </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
       <c r="E7" t="s">
         <v>38</v>
       </c>
@@ -659,6 +659,9 @@
       <c r="C13" t="s">
         <v>37</v>
       </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -670,6 +673,9 @@
       <c r="C14" t="s">
         <v>37</v>
       </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -681,6 +687,9 @@
       <c r="C15" t="s">
         <v>37</v>
       </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -692,8 +701,11 @@
       <c r="C16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -701,10 +713,13 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -714,8 +729,11 @@
       <c r="C18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -725,8 +743,11 @@
       <c r="C19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -734,6 +755,9 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>